<commit_message>
compare tab and site gps file  fixed
</commit_message>
<xml_diff>
--- a/data/site gps.xlsx
+++ b/data/site gps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorisliu/Github/Outreach-Fall-ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorisliu/Github/Outreach_Fall_ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5FE7DA-577C-AF40-AFE7-F047592BA06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B014AFE-F760-D249-875D-FBAF2B08998C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{A3D63D45-D1DF-5D47-A658-FB95F610A03E}"/>
+    <workbookView xWindow="11160" yWindow="500" windowWidth="17260" windowHeight="14900" xr2:uid="{A3D63D45-D1DF-5D47-A658-FB95F610A03E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,19 +484,25 @@
         <v>-120.27191157990499</v>
       </c>
       <c r="D2">
-        <v>8.099729</v>
+        <v>7.95</v>
       </c>
       <c r="E2">
-        <v>16.05048</v>
+        <v>16.760000000000002</v>
       </c>
       <c r="F2">
         <v>3.2541929999999999</v>
       </c>
+      <c r="G2">
+        <v>8.2330000000000005</v>
+      </c>
+      <c r="H2">
+        <v>7.2690000000000001</v>
+      </c>
       <c r="I2">
-        <v>19.779630000000001</v>
+        <v>20.53</v>
       </c>
       <c r="J2">
-        <v>11.08048</v>
+        <v>11.69</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -510,25 +516,25 @@
         <v>-123.072185569311</v>
       </c>
       <c r="D3">
-        <v>7.8982190000000001</v>
+        <v>7.8940000000000001</v>
       </c>
       <c r="E3">
-        <v>13.74967</v>
+        <v>13.46</v>
       </c>
       <c r="F3">
         <v>4.2774599999999996</v>
       </c>
       <c r="G3">
-        <v>8.4071339999999992</v>
+        <v>8.532</v>
       </c>
       <c r="H3">
-        <v>7.4660299999999999</v>
+        <v>7.5010000000000003</v>
       </c>
       <c r="I3">
-        <v>16.517430000000001</v>
+        <v>22.239000000000001</v>
       </c>
       <c r="J3">
-        <v>8.457789</v>
+        <v>6.3330000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -542,25 +548,25 @@
         <v>-120.600513452637</v>
       </c>
       <c r="D4">
-        <v>7.9660510000000002</v>
+        <v>7.8490000000000002</v>
       </c>
       <c r="E4">
-        <v>12.907030000000001</v>
+        <v>14.63</v>
       </c>
       <c r="F4">
         <v>3.3599239999999999</v>
       </c>
       <c r="G4">
-        <v>8.2683949999999999</v>
+        <v>8.2490000000000006</v>
       </c>
       <c r="H4">
-        <v>7.6204010000000002</v>
+        <v>7.1790000000000003</v>
       </c>
       <c r="I4">
-        <v>19.246459999999999</v>
+        <v>22.88</v>
       </c>
       <c r="J4">
-        <v>10.382580000000001</v>
+        <v>11.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean up data_summary_table for compare/contrast, brute force add radius differences
</commit_message>
<xml_diff>
--- a/data/site gps.xlsx
+++ b/data/site gps.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorisliu/Github/Outreach_Fall_ShinyApp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amelia/github/Outreach-Fall-ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B014AFE-F760-D249-875D-FBAF2B08998C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8741E0B-0CE7-D34D-8641-2C6CCC87418F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="500" windowWidth="17260" windowHeight="14900" xr2:uid="{A3D63D45-D1DF-5D47-A658-FB95F610A03E}"/>
+    <workbookView xWindow="17360" yWindow="500" windowWidth="12240" windowHeight="14900" xr2:uid="{A3D63D45-D1DF-5D47-A658-FB95F610A03E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -435,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABC61E6-BDEB-3442-A378-2D6D5E0939D9}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,25 +485,25 @@
         <v>-120.27191157990499</v>
       </c>
       <c r="D2">
-        <v>7.95</v>
+        <v>7.98</v>
       </c>
       <c r="E2">
-        <v>16.760000000000002</v>
+        <v>17.27</v>
       </c>
       <c r="F2">
         <v>3.2541929999999999</v>
       </c>
       <c r="G2">
-        <v>8.2330000000000005</v>
+        <v>8.23</v>
       </c>
       <c r="H2">
-        <v>7.2690000000000001</v>
+        <v>7.63</v>
       </c>
       <c r="I2">
         <v>20.53</v>
       </c>
       <c r="J2">
-        <v>11.69</v>
+        <v>14.06</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -516,25 +517,25 @@
         <v>-123.072185569311</v>
       </c>
       <c r="D3">
-        <v>7.8940000000000001</v>
+        <v>7.89</v>
       </c>
       <c r="E3">
-        <v>13.46</v>
+        <v>13.92</v>
       </c>
       <c r="F3">
         <v>4.2774599999999996</v>
       </c>
       <c r="G3">
-        <v>8.532</v>
+        <v>8.27</v>
       </c>
       <c r="H3">
-        <v>7.5010000000000003</v>
+        <v>7.5</v>
       </c>
       <c r="I3">
-        <v>22.239000000000001</v>
+        <v>17.18</v>
       </c>
       <c r="J3">
-        <v>6.3330000000000002</v>
+        <v>10.01</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -548,25 +549,25 @@
         <v>-120.600513452637</v>
       </c>
       <c r="D4">
-        <v>7.8490000000000002</v>
+        <v>7.93</v>
       </c>
       <c r="E4">
-        <v>14.63</v>
+        <v>14.36</v>
       </c>
       <c r="F4">
         <v>3.3599239999999999</v>
       </c>
       <c r="G4">
-        <v>8.2490000000000006</v>
+        <v>8.25</v>
       </c>
       <c r="H4">
-        <v>7.1790000000000003</v>
+        <v>7.28</v>
       </c>
       <c r="I4">
         <v>22.88</v>
       </c>
       <c r="J4">
-        <v>11.07</v>
+        <v>11.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>